<commit_message>
second commit file3 in seinur
</commit_message>
<xml_diff>
--- a/file3.xlsx
+++ b/file3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DCBF09-BA8C-439B-9F90-314F95B4E6F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +54,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +331,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <f>SUM(A5,C5)</f>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>123</v>
+      </c>
+      <c r="C5">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit gitignore and otkat
</commit_message>
<xml_diff>
--- a/file3.xlsx
+++ b/file3.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DCBF09-BA8C-439B-9F90-314F95B4E6F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -54,7 +53,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -331,30 +330,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <f>SUM(A5,C5)</f>
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>123</v>
-      </c>
-      <c r="C5">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>